<commit_message>
feat: unit test of incident
</commit_message>
<xml_diff>
--- a/data/incidents.xlsx
+++ b/data/incidents.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I999"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8485,6 +8485,44 @@
         <v/>
       </c>
     </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>3e572f1e-c6a8-41ea-b21b-28acdd585cdf</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>R001</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>Riku</t>
+        </is>
+      </c>
+      <c r="D1000" t="inlineStr">
+        <is>
+          <t>Traffic</t>
+        </is>
+      </c>
+      <c r="E1000" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="F1000" s="4" t="n">
+        <v>45820.67373396213</v>
+      </c>
+      <c r="G1000" s="4" t="n">
+        <v>45820.7154006288</v>
+      </c>
+      <c r="H1000" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I1000">
     <cfRule type="expression" priority="1" dxfId="0">

</xml_diff>